<commit_message>
Started working on everything
Want to get things done by Monday
</commit_message>
<xml_diff>
--- a/Documentation/flrTravelDistance.xlsx
+++ b/Documentation/flrTravelDistance.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8CBB7F-2C5B-46D9-822E-EEF991E1020A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,8 +112,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{AE10B387-1B8B-4B70-86E7-84B350072E02}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -386,29 +415,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -449,7 +478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>101</v>
       </c>
@@ -462,11 +491,11 @@
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>0.5625</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -477,14 +506,14 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>2.75</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>2.25</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -497,13 +526,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="5">
+      <c r="D5" s="2">
         <v>1.0625</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -513,23 +542,23 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <v>0.5</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -542,7 +571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -556,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>102</v>
       </c>
@@ -571,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -587,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -604,7 +633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>87</v>
       </c>
@@ -622,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/minx112/Fallout-Live-radio"
This reverts commit fd28234af129807ef36af9760236b1005caa0602, reversing
changes made to bc22710a35e519bd5d28989ace5b2c6bce4f4a25.
</commit_message>
<xml_diff>
--- a/Documentation/flrTravelDistance.xlsx
+++ b/Documentation/flrTravelDistance.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8CBB7F-2C5B-46D9-822E-EEF991E1020A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,36 +111,8 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{AE10B387-1B8B-4B70-86E7-84B350072E02}">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -415,29 +386,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" customWidth="1"/>
-    <col min="11" max="11" width="5.42578125" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" customWidth="1"/>
+    <col min="11" max="11" width="5.44140625" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -478,7 +449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>101</v>
       </c>
@@ -491,11 +462,11 @@
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>0.5625</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -506,14 +477,14 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>2.75</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>2.25</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -526,13 +497,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>1.0625</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -542,23 +513,23 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>0.5</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -571,7 +542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -585,7 +556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>102</v>
       </c>
@@ -600,7 +571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -616,7 +587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -633,7 +604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>87</v>
       </c>
@@ -651,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/minx112/Fallout-Live-radio""
This reverts commit 356a7d3b2ca6a915f81b26b22600fbbbcfd69d85.
</commit_message>
<xml_diff>
--- a/Documentation/flrTravelDistance.xlsx
+++ b/Documentation/flrTravelDistance.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8CBB7F-2C5B-46D9-822E-EEF991E1020A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,8 +112,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{AE10B387-1B8B-4B70-86E7-84B350072E02}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -386,29 +415,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -449,7 +478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>101</v>
       </c>
@@ -462,11 +491,11 @@
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>0.5625</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -477,14 +506,14 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>2.75</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>2.25</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -497,13 +526,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="5">
+      <c r="D5" s="2">
         <v>1.0625</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -513,23 +542,23 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <v>0.5</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -542,7 +571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -556,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>102</v>
       </c>
@@ -571,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
@@ -587,7 +616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -604,7 +633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>87</v>
       </c>
@@ -622,7 +651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>

</xml_diff>